<commit_message>
Fixing the bug for q5
It was because movies was not sorted
</commit_message>
<xml_diff>
--- a/assignment4/q5_data.xlsx
+++ b/assignment4/q5_data.xlsx
@@ -446,67 +446,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>M4</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>M8</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>M9</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>M12</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>M6</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>M13</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>M14</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>M3</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>M7</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>M11</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>M5</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>M7</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>M8</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>M11</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>M14</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>M1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>M4</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>M6</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>M9</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>M12</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>M13</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -525,23 +525,21 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -558,41 +556,35 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="n">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -602,41 +594,39 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" t="n">
-        <v>3</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>2</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -648,39 +638,37 @@
       <c r="B5" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -693,37 +681,41 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>2</v>
       </c>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -732,39 +724,33 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
+      <c r="J7" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>5</v>
       </c>
-      <c r="M7" t="n">
-        <v>3</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="n">
-        <v>3</v>
-      </c>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -774,35 +760,37 @@
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
       <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
       <c r="M8" t="n">
-        <v>2</v>
-      </c>
-      <c r="N8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O8" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>4</v>
+      </c>
       <c r="P8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -812,38 +800,36 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>5</v>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>4</v>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
-        <v>3</v>
-      </c>
-      <c r="N9" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>3</v>
+      </c>
       <c r="O9" t="n">
         <v>3</v>
       </c>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -852,17 +838,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
       <c r="E10" t="n">
         <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
         <v>3</v>
@@ -871,21 +859,19 @@
         <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>3</v>
-      </c>
-      <c r="P10" t="n">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -894,34 +880,32 @@
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" t="n">
-        <v>5</v>
-      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2</v>
+      </c>
       <c r="L11" t="n">
         <v>1</v>
       </c>
-      <c r="M11" t="n">
-        <v>2</v>
-      </c>
-      <c r="N11" t="n">
-        <v>3</v>
-      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>2</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>